<commit_message>
Simulations chap1/2 in new format
</commit_message>
<xml_diff>
--- a/Measurements/Chapter 2 - Cumulative error.xlsx
+++ b/Measurements/Chapter 2 - Cumulative error.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28635" windowHeight="12600" tabRatio="1000"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="28635" windowHeight="12600" tabRatio="1000" firstSheet="3" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="k=160" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="206">
   <si>
     <t>Time</t>
   </si>
@@ -51,6 +51,606 @@
   </si>
   <si>
     <t>Result</t>
+  </si>
+  <si>
+    <t>(0, 0.96)</t>
+  </si>
+  <si>
+    <t>(1, 0.384)</t>
+  </si>
+  <si>
+    <t>(2, 0.7295999999999999)</t>
+  </si>
+  <si>
+    <t>(3, 0.52224)</t>
+  </si>
+  <si>
+    <t>(4, 0.646656)</t>
+  </si>
+  <si>
+    <t>(5, 0.5720063999999999)</t>
+  </si>
+  <si>
+    <t>(6, 0.6167961599999999)</t>
+  </si>
+  <si>
+    <t>(7, 0.5899223040000001)</t>
+  </si>
+  <si>
+    <t>(8, 0.6060466175999999)</t>
+  </si>
+  <si>
+    <t>(9, 0.5963720294399999)</t>
+  </si>
+  <si>
+    <t>(10, 0.6021767823360001)</t>
+  </si>
+  <si>
+    <t>(11, 0.5986939305983998)</t>
+  </si>
+  <si>
+    <t>(12, 0.6007836416409602)</t>
+  </si>
+  <si>
+    <t>(13, 0.5995298150154238)</t>
+  </si>
+  <si>
+    <t>(14, 0.6002821109907457)</t>
+  </si>
+  <si>
+    <t>(15, 0.5998307334055525)</t>
+  </si>
+  <si>
+    <t>(16, 0.6001015599566685)</t>
+  </si>
+  <si>
+    <t>(17, 0.599939064025999)</t>
+  </si>
+  <si>
+    <t>(18, 0.6000365615844006)</t>
+  </si>
+  <si>
+    <t>(19, 0.5999780630493596)</t>
+  </si>
+  <si>
+    <t>(20, 0.6000131621703843)</t>
+  </si>
+  <si>
+    <t>(21, 0.5999921026977694)</t>
+  </si>
+  <si>
+    <t>(22, 0.6000047383813383)</t>
+  </si>
+  <si>
+    <t>(23, 0.599997156971197)</t>
+  </si>
+  <si>
+    <t>(24, 0.6000017058172817)</t>
+  </si>
+  <si>
+    <t>(25, 0.599998976509631)</t>
+  </si>
+  <si>
+    <t>(26, 0.6000006140942213)</t>
+  </si>
+  <si>
+    <t>(27, 0.5999996315434671)</t>
+  </si>
+  <si>
+    <t>(28, 0.6000002210739197)</t>
+  </si>
+  <si>
+    <t>(29, 0.5999998673556481)</t>
+  </si>
+  <si>
+    <t>(30, 0.6000000795866111)</t>
+  </si>
+  <si>
+    <t>(31, 0.5999999522480334)</t>
+  </si>
+  <si>
+    <t>(32, 0.60000002865118)</t>
+  </si>
+  <si>
+    <t>(33, 0.5999999828092919)</t>
+  </si>
+  <si>
+    <t>(34, 0.6000000103144248)</t>
+  </si>
+  <si>
+    <t>(35, 0.5999999938113451)</t>
+  </si>
+  <si>
+    <t>(36, 0.600000003713193)</t>
+  </si>
+  <si>
+    <t>(37, 0.5999999977720841)</t>
+  </si>
+  <si>
+    <t>(38, 0.6000000013367496)</t>
+  </si>
+  <si>
+    <t>(39, 0.5999999991979501)</t>
+  </si>
+  <si>
+    <t>(40, 0.60000000048123)</t>
+  </si>
+  <si>
+    <t>(41, 0.5999999997112618)</t>
+  </si>
+  <si>
+    <t>(42, 0.600000000173243)</t>
+  </si>
+  <si>
+    <t>(43, 0.5999999998960541)</t>
+  </si>
+  <si>
+    <t>(44, 0.6000000000623675)</t>
+  </si>
+  <si>
+    <t>(45, 0.5999999999625794)</t>
+  </si>
+  <si>
+    <t>(46, 0.6000000000224525)</t>
+  </si>
+  <si>
+    <t>(47, 0.5999999999865284)</t>
+  </si>
+  <si>
+    <t>(48, 0.600000000008083)</t>
+  </si>
+  <si>
+    <t>(49, 0.5999999999951502)</t>
+  </si>
+  <si>
+    <t>(50, 0.9200000000029099)</t>
+  </si>
+  <si>
+    <t>(51, 0.7279999999982542)</t>
+  </si>
+  <si>
+    <t>(52, 0.8432000000010476)</t>
+  </si>
+  <si>
+    <t>(53, 0.7740799999993715)</t>
+  </si>
+  <si>
+    <t>(54, 0.8155520000003773)</t>
+  </si>
+  <si>
+    <t>(55, 0.7906687999997736)</t>
+  </si>
+  <si>
+    <t>(56, 0.805598720000136)</t>
+  </si>
+  <si>
+    <t>(57, 0.7966407679999185)</t>
+  </si>
+  <si>
+    <t>(58, 0.802015539200049)</t>
+  </si>
+  <si>
+    <t>(59, 0.7987906764799706)</t>
+  </si>
+  <si>
+    <t>(60, 0.8007255941120178)</t>
+  </si>
+  <si>
+    <t>(61, 0.7995646435327893)</t>
+  </si>
+  <si>
+    <t>(62, 0.8002612138803264)</t>
+  </si>
+  <si>
+    <t>(63, 0.7998432716718042)</t>
+  </si>
+  <si>
+    <t>(64, 0.8000940369969175)</t>
+  </si>
+  <si>
+    <t>(65, 0.7999435778018495)</t>
+  </si>
+  <si>
+    <t>(66, 0.8000338533188903)</t>
+  </si>
+  <si>
+    <t>(67, 0.799979688008666)</t>
+  </si>
+  <si>
+    <t>(68, 0.8000121871948004)</t>
+  </si>
+  <si>
+    <t>(69, 0.7999926876831198)</t>
+  </si>
+  <si>
+    <t>(70, 0.8000043873901282)</t>
+  </si>
+  <si>
+    <t>(71, 0.7999973675659231)</t>
+  </si>
+  <si>
+    <t>(72, 0.8000015794604463)</t>
+  </si>
+  <si>
+    <t>(73, 0.7999990523237323)</t>
+  </si>
+  <si>
+    <t>(74, 0.8000005686057606)</t>
+  </si>
+  <si>
+    <t>(75, 0.7999996588365437)</t>
+  </si>
+  <si>
+    <t>(76, 0.800000204698074)</t>
+  </si>
+  <si>
+    <t>(77, 0.7999998771811556)</t>
+  </si>
+  <si>
+    <t>(78, 0.8000000736913067)</t>
+  </si>
+  <si>
+    <t>(79, 0.7999999557852162)</t>
+  </si>
+  <si>
+    <t>(80, 0.8000000265288704)</t>
+  </si>
+  <si>
+    <t>(81, 0.7999999840826777)</t>
+  </si>
+  <si>
+    <t>(82, 0.8000000095503935)</t>
+  </si>
+  <si>
+    <t>(83, 0.799999994269764)</t>
+  </si>
+  <si>
+    <t>(84, 0.8000000034381416)</t>
+  </si>
+  <si>
+    <t>(85, 0.7999999979371153)</t>
+  </si>
+  <si>
+    <t>(86, 0.8000000012377307)</t>
+  </si>
+  <si>
+    <t>(87, 0.7999999992573618)</t>
+  </si>
+  <si>
+    <t>(88, 0.800000000445583)</t>
+  </si>
+  <si>
+    <t>(89, 0.7999999997326503)</t>
+  </si>
+  <si>
+    <t>(90, 0.8000000001604098)</t>
+  </si>
+  <si>
+    <t>(91, 0.7999999999037541)</t>
+  </si>
+  <si>
+    <t>(92, 0.8000000000577475)</t>
+  </si>
+  <si>
+    <t>(93, 0.7999999999653516)</t>
+  </si>
+  <si>
+    <t>(94, 0.8000000000207891)</t>
+  </si>
+  <si>
+    <t>(95, 0.7999999999875266)</t>
+  </si>
+  <si>
+    <t>(96, 0.8000000000074842)</t>
+  </si>
+  <si>
+    <t>(97, 0.7999999999955095)</t>
+  </si>
+  <si>
+    <t>(98, 0.8000000000026943)</t>
+  </si>
+  <si>
+    <t>(99, 0.7999999999983836)</t>
+  </si>
+  <si>
+    <t>(100, 0.0)</t>
+  </si>
+  <si>
+    <t>(101, 0.0)</t>
+  </si>
+  <si>
+    <t>(102, 9.698020164705668E-13)</t>
+  </si>
+  <si>
+    <t>(103, 0.1599999999994181)</t>
+  </si>
+  <si>
+    <t>(104, 0.06400000000034915)</t>
+  </si>
+  <si>
+    <t>(105, 0.12159999999979051)</t>
+  </si>
+  <si>
+    <t>(106, 0.0870400000001257)</t>
+  </si>
+  <si>
+    <t>(107, 0.10777599999992461)</t>
+  </si>
+  <si>
+    <t>(108, 0.09533440000004523)</t>
+  </si>
+  <si>
+    <t>(109, 0.10279935999997286)</t>
+  </si>
+  <si>
+    <t>(110, 0.0983203840000163)</t>
+  </si>
+  <si>
+    <t>(111, 0.10100776959999022)</t>
+  </si>
+  <si>
+    <t>(112, 0.09939533824000588)</t>
+  </si>
+  <si>
+    <t>(113, 0.10036279705599649)</t>
+  </si>
+  <si>
+    <t>(114, 0.09978232176640212)</t>
+  </si>
+  <si>
+    <t>(115, 0.10013060694015874)</t>
+  </si>
+  <si>
+    <t>(116, 0.09992163583590477)</t>
+  </si>
+  <si>
+    <t>(117, 0.10004701849845715)</t>
+  </si>
+  <si>
+    <t>(118, 0.0999717889009257)</t>
+  </si>
+  <si>
+    <t>(119, 0.10001692665944459)</t>
+  </si>
+  <si>
+    <t>(120, 0.09998984400433325)</t>
+  </si>
+  <si>
+    <t>(121, 0.10000609359740008)</t>
+  </si>
+  <si>
+    <t>(122, 0.09999634384155996)</t>
+  </si>
+  <si>
+    <t>(123, 0.10000219369506402)</t>
+  </si>
+  <si>
+    <t>(124, 0.0999986837829616)</t>
+  </si>
+  <si>
+    <t>(125, 0.10000078973022304)</t>
+  </si>
+  <si>
+    <t>(126, 0.09999952616186619)</t>
+  </si>
+  <si>
+    <t>(127, 0.10000028430288027)</t>
+  </si>
+  <si>
+    <t>(128, 0.09999982941827186)</t>
+  </si>
+  <si>
+    <t>(129, 0.10000010234903689)</t>
+  </si>
+  <si>
+    <t>(130, 0.09999993859057789)</t>
+  </si>
+  <si>
+    <t>(131, 0.10000003684565327)</t>
+  </si>
+  <si>
+    <t>(132, 0.09999997789260803)</t>
+  </si>
+  <si>
+    <t>(133, 0.10000001326443521)</t>
+  </si>
+  <si>
+    <t>(134, 0.09999999204133887)</t>
+  </si>
+  <si>
+    <t>(135, 0.10000000477519669)</t>
+  </si>
+  <si>
+    <t>(136, 0.09999999713488199)</t>
+  </si>
+  <si>
+    <t>(137, 0.10000000171907082)</t>
+  </si>
+  <si>
+    <t>(138, 0.09999999896855752)</t>
+  </si>
+  <si>
+    <t>(139, 0.10000000061886549)</t>
+  </si>
+  <si>
+    <t>(140, 0.09999999962868071)</t>
+  </si>
+  <si>
+    <t>(141, 0.10000000022279158)</t>
+  </si>
+  <si>
+    <t>(142, 0.09999999986632506)</t>
+  </si>
+  <si>
+    <t>(143, 0.10000000008020499)</t>
+  </si>
+  <si>
+    <t>(144, 0.099999999951877)</t>
+  </si>
+  <si>
+    <t>(145, 0.10000000002887381)</t>
+  </si>
+  <si>
+    <t>(146, 0.09999999998267572)</t>
+  </si>
+  <si>
+    <t>(147, 0.10000000001039457)</t>
+  </si>
+  <si>
+    <t>(148, 0.09999999999376329)</t>
+  </si>
+  <si>
+    <t>(149, 0.10000000000374204)</t>
+  </si>
+  <si>
+    <t>(150, 1.0)</t>
+  </si>
+  <si>
+    <t>(151, 1.0)</t>
+  </si>
+  <si>
+    <t>(152, 1.0)</t>
+  </si>
+  <si>
+    <t>(153, 0.8999999999977548)</t>
+  </si>
+  <si>
+    <t>(154, 0.9000000000013472)</t>
+  </si>
+  <si>
+    <t>(155, 0.8999999999991917)</t>
+  </si>
+  <si>
+    <t>(156, 0.9000000000004852)</t>
+  </si>
+  <si>
+    <t>(157, 0.8999999999997088)</t>
+  </si>
+  <si>
+    <t>(158, 0.9000000000001748)</t>
+  </si>
+  <si>
+    <t>(159, 0.8999999999998951)</t>
+  </si>
+  <si>
+    <t>(160, 0.9000000000000631)</t>
+  </si>
+  <si>
+    <t>(161, 0.8999999999999622)</t>
+  </si>
+  <si>
+    <t>(162, 0.9000000000000228)</t>
+  </si>
+  <si>
+    <t>(163, 0.8999999999999864)</t>
+  </si>
+  <si>
+    <t>(164, 0.9000000000000082)</t>
+  </si>
+  <si>
+    <t>(165, 0.899999999999995)</t>
+  </si>
+  <si>
+    <t>(166, 0.900000000000003)</t>
+  </si>
+  <si>
+    <t>(167, 0.8999999999999982)</t>
+  </si>
+  <si>
+    <t>(168, 0.9000000000000011)</t>
+  </si>
+  <si>
+    <t>(169, 0.8999999999999992)</t>
+  </si>
+  <si>
+    <t>(170, 0.9000000000000006)</t>
+  </si>
+  <si>
+    <t>(171, 0.8999999999999997)</t>
+  </si>
+  <si>
+    <t>(172, 0.9000000000000001)</t>
+  </si>
+  <si>
+    <t>(173, 0.9)</t>
+  </si>
+  <si>
+    <t>(174, 0.9)</t>
+  </si>
+  <si>
+    <t>(175, 0.9)</t>
+  </si>
+  <si>
+    <t>(176, 0.9)</t>
+  </si>
+  <si>
+    <t>(177, 0.9)</t>
+  </si>
+  <si>
+    <t>(178, 0.9)</t>
+  </si>
+  <si>
+    <t>(179, 0.9)</t>
+  </si>
+  <si>
+    <t>(180, 0.9)</t>
+  </si>
+  <si>
+    <t>(181, 0.9)</t>
+  </si>
+  <si>
+    <t>(182, 0.9)</t>
+  </si>
+  <si>
+    <t>(183, 0.9)</t>
+  </si>
+  <si>
+    <t>(184, 0.9)</t>
+  </si>
+  <si>
+    <t>(185, 0.9)</t>
+  </si>
+  <si>
+    <t>(186, 0.9)</t>
+  </si>
+  <si>
+    <t>(187, 0.9)</t>
+  </si>
+  <si>
+    <t>(188, 0.9)</t>
+  </si>
+  <si>
+    <t>(189, 0.9)</t>
+  </si>
+  <si>
+    <t>(190, 0.9)</t>
+  </si>
+  <si>
+    <t>(191, 0.9)</t>
+  </si>
+  <si>
+    <t>(192, 0.9)</t>
+  </si>
+  <si>
+    <t>(193, 0.9)</t>
+  </si>
+  <si>
+    <t>(194, 0.9)</t>
+  </si>
+  <si>
+    <t>(195, 0.9)</t>
+  </si>
+  <si>
+    <t>(196, 0.9)</t>
+  </si>
+  <si>
+    <t>(197, 0.9)</t>
+  </si>
+  <si>
+    <t>(198, 0.9)</t>
+  </si>
+  <si>
+    <t>(199, 0.9)</t>
   </si>
 </sst>
 </file>
@@ -1379,11 +1979,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="133870720"/>
-        <c:axId val="133872640"/>
+        <c:axId val="118979968"/>
+        <c:axId val="119571968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="133870720"/>
+        <c:axId val="118979968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -1413,12 +2013,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133872640"/>
+        <c:crossAx val="119571968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133872640"/>
+        <c:axId val="119571968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1448,7 +2048,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133870720"/>
+        <c:crossAx val="118979968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2743,11 +3343,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="134526080"/>
-        <c:axId val="134528000"/>
+        <c:axId val="121220096"/>
+        <c:axId val="121468032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="134526080"/>
+        <c:axId val="121220096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -2776,12 +3376,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134528000"/>
+        <c:crossAx val="121468032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="134528000"/>
+        <c:axId val="121468032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2810,7 +3410,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134526080"/>
+        <c:crossAx val="121220096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4090,11 +4690,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="134536576"/>
-        <c:axId val="134579712"/>
+        <c:axId val="121374208"/>
+        <c:axId val="121376128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="134536576"/>
+        <c:axId val="121374208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -4123,12 +4723,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134579712"/>
+        <c:crossAx val="121376128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="134579712"/>
+        <c:axId val="121376128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4157,7 +4757,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134536576"/>
+        <c:crossAx val="121374208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4204,6 +4804,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6694,11 +7295,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="134703744"/>
-        <c:axId val="134710016"/>
+        <c:axId val="121537280"/>
+        <c:axId val="121539200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="134703744"/>
+        <c:axId val="121537280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -6721,18 +7322,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134710016"/>
+        <c:crossAx val="121539200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="134710016"/>
+        <c:axId val="121539200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -6757,19 +7359,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134703744"/>
+        <c:crossAx val="121537280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6794,6 +7398,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -8047,11 +8652,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="135026176"/>
-        <c:axId val="135028096"/>
+        <c:axId val="121548160"/>
+        <c:axId val="121681408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="135026176"/>
+        <c:axId val="121548160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -8074,18 +8679,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135028096"/>
+        <c:crossAx val="121681408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="135028096"/>
+        <c:axId val="121681408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8108,13 +8714,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135026176"/>
+        <c:crossAx val="121548160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8156,6 +8763,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -9409,11 +10017,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="136323072"/>
-        <c:axId val="136324992"/>
+        <c:axId val="120465280"/>
+        <c:axId val="120471552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="136323072"/>
+        <c:axId val="120465280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -9436,18 +10044,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136324992"/>
+        <c:crossAx val="120471552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="136324992"/>
+        <c:axId val="120471552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9470,13 +10079,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136323072"/>
+        <c:crossAx val="120465280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9503,6 +10113,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -10756,11 +11367,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="137844992"/>
-        <c:axId val="145977728"/>
+        <c:axId val="121061760"/>
+        <c:axId val="121063680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="137844992"/>
+        <c:axId val="121061760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -10783,18 +11394,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145977728"/>
+        <c:crossAx val="121063680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="145977728"/>
+        <c:axId val="121063680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10817,13 +11429,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137844992"/>
+        <c:crossAx val="121061760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13361,11 +13974,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="147854848"/>
-        <c:axId val="147856768"/>
+        <c:axId val="121085312"/>
+        <c:axId val="121112064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="147854848"/>
+        <c:axId val="121085312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -13395,12 +14008,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147856768"/>
+        <c:crossAx val="121112064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="147856768"/>
+        <c:axId val="121112064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -13432,7 +14045,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147854848"/>
+        <c:crossAx val="121085312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13479,6 +14092,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -14732,11 +15346,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="133959040"/>
-        <c:axId val="133998080"/>
+        <c:axId val="120174464"/>
+        <c:axId val="120176640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="133959040"/>
+        <c:axId val="120174464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -14759,18 +15373,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133998080"/>
+        <c:crossAx val="120176640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133998080"/>
+        <c:axId val="120176640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14793,13 +15408,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133959040"/>
+        <c:crossAx val="120174464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14826,6 +15442,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -16079,11 +16696,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="134010752"/>
-        <c:axId val="134017024"/>
+        <c:axId val="120078720"/>
+        <c:axId val="120080640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="134010752"/>
+        <c:axId val="120078720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -16106,18 +16723,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134017024"/>
+        <c:crossAx val="120080640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="134017024"/>
+        <c:axId val="120080640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16140,13 +16758,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134010752"/>
+        <c:crossAx val="120078720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -16193,6 +16812,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -18683,11 +19303,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="134075520"/>
-        <c:axId val="134077440"/>
+        <c:axId val="120813056"/>
+        <c:axId val="120814976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="134075520"/>
+        <c:axId val="120813056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -18710,18 +19330,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134077440"/>
+        <c:crossAx val="120814976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="134077440"/>
+        <c:axId val="120814976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -18746,19 +19367,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134075520"/>
+        <c:crossAx val="120813056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -20036,11 +20659,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="134135808"/>
-        <c:axId val="134137728"/>
+        <c:axId val="120889344"/>
+        <c:axId val="120891264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="134135808"/>
+        <c:axId val="120889344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -20069,12 +20692,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134137728"/>
+        <c:crossAx val="120891264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="134137728"/>
+        <c:axId val="120891264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20103,7 +20726,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134135808"/>
+        <c:crossAx val="120889344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -21398,11 +22021,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="134158592"/>
-        <c:axId val="134168960"/>
+        <c:axId val="120736000"/>
+        <c:axId val="120738176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="134158592"/>
+        <c:axId val="120736000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -21431,12 +22054,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134168960"/>
+        <c:crossAx val="120738176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="134168960"/>
+        <c:axId val="120738176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21465,7 +22088,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134158592"/>
+        <c:crossAx val="120736000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -22745,11 +23368,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="134263552"/>
-        <c:axId val="134265472"/>
+        <c:axId val="120097792"/>
+        <c:axId val="120566912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="134263552"/>
+        <c:axId val="120097792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -22778,12 +23401,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134265472"/>
+        <c:crossAx val="120566912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="134265472"/>
+        <c:axId val="120566912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22812,7 +23435,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134263552"/>
+        <c:crossAx val="120097792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -25349,11 +25972,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="134311936"/>
-        <c:axId val="134313856"/>
+        <c:axId val="121248000"/>
+        <c:axId val="121250176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="134311936"/>
+        <c:axId val="121248000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -25382,12 +26005,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134313856"/>
+        <c:crossAx val="121250176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="134313856"/>
+        <c:axId val="121250176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -25418,7 +26041,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134311936"/>
+        <c:crossAx val="121248000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -26702,11 +27325,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="134355584"/>
-        <c:axId val="134382336"/>
+        <c:axId val="121197312"/>
+        <c:axId val="121199232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="134355584"/>
+        <c:axId val="121197312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -26735,12 +27358,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134382336"/>
+        <c:crossAx val="121199232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="134382336"/>
+        <c:axId val="121199232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26769,7 +27392,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134355584"/>
+        <c:crossAx val="121197312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -26862,7 +27485,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="129" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="129" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -27678,7 +28301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -39794,11 +40417,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F201"/>
+  <dimension ref="A1:H201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -39806,7 +40429,7 @@
     <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -39826,7 +40449,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -39845,8 +40468,11 @@
       <c r="F2" s="2">
         <v>0.96</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -39865,8 +40491,11 @@
       <c r="F3" s="2">
         <v>0.38400000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -39885,8 +40514,11 @@
       <c r="F4" s="2">
         <v>0.72959999999999903</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -39905,8 +40537,11 @@
       <c r="F5" s="2">
         <v>0.52224000000000004</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -39925,8 +40560,11 @@
       <c r="F6" s="2">
         <v>0.64665600000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -39945,8 +40583,11 @@
       <c r="F7" s="2">
         <v>0.57200639999999903</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -39965,8 +40606,11 @@
       <c r="F8" s="2">
         <v>0.61679615999999904</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -39985,8 +40629,11 @@
       <c r="F9" s="2">
         <v>0.58992230400000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -40005,8 +40652,11 @@
       <c r="F10" s="2">
         <v>0.606046617599999</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -40025,8 +40675,11 @@
       <c r="F11" s="2">
         <v>0.59637202943999901</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -40045,8 +40698,11 @@
       <c r="F12" s="2">
         <v>0.60217678233600003</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -40065,8 +40721,11 @@
       <c r="F13" s="2">
         <v>0.59869393059839904</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -40085,8 +40744,11 @@
       <c r="F14" s="2">
         <v>0.60078364164095999</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -40105,8 +40767,11 @@
       <c r="F15" s="2">
         <v>0.59952981501542302</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -40125,8 +40790,11 @@
       <c r="F16" s="2">
         <v>0.60028211099074502</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -40145,8 +40813,11 @@
       <c r="F17" s="2">
         <v>0.59983073340555204</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -40165,8 +40836,11 @@
       <c r="F18" s="2">
         <v>0.60010155995666803</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -40185,8 +40859,11 @@
       <c r="F19" s="2">
         <v>0.59993906402599895</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -40205,8 +40882,11 @@
       <c r="F20" s="2">
         <v>0.6000365615844</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -40225,8 +40905,11 @@
       <c r="F21" s="2">
         <v>0.59997806304935897</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -40245,8 +40928,11 @@
       <c r="F22" s="2">
         <v>0.60001316217038403</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -40265,8 +40951,11 @@
       <c r="F23" s="2">
         <v>0.59999210269776904</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -40285,8 +40974,11 @@
       <c r="F24" s="2">
         <v>0.60000473838133805</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -40305,8 +40997,11 @@
       <c r="F25" s="2">
         <v>0.59999715697119704</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -40325,8 +41020,11 @@
       <c r="F26" s="2">
         <v>0.60000170581728096</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -40345,8 +41043,11 @@
       <c r="F27" s="2">
         <v>0.59999897650963097</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -40365,8 +41066,11 @@
       <c r="F28" s="2">
         <v>0.60000061409422101</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -40385,8 +41089,11 @@
       <c r="F29" s="2">
         <v>0.59999963154346703</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -40405,8 +41112,11 @@
       <c r="F30" s="2">
         <v>0.60000022107391904</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -40425,8 +41135,11 @@
       <c r="F31" s="2">
         <v>0.59999986735564803</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -40445,8 +41158,11 @@
       <c r="F32" s="2">
         <v>0.60000007958661095</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -40465,8 +41181,11 @@
       <c r="F33" s="2">
         <v>0.59999995224803304</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -40485,8 +41204,11 @@
       <c r="F34" s="2">
         <v>0.60000002865117996</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>33</v>
       </c>
@@ -40505,8 +41227,11 @@
       <c r="F35" s="2">
         <v>0.59999998280929101</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -40525,8 +41250,11 @@
       <c r="F36" s="2">
         <v>0.60000001031442396</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>35</v>
       </c>
@@ -40545,8 +41273,11 @@
       <c r="F37" s="2">
         <v>0.59999999381134494</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>36</v>
       </c>
@@ -40565,8 +41296,11 @@
       <c r="F38" s="2">
         <v>0.60000000371319295</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>37</v>
       </c>
@@ -40585,8 +41319,11 @@
       <c r="F39" s="2">
         <v>0.59999999777208401</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H39" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>38</v>
       </c>
@@ -40605,8 +41342,11 @@
       <c r="F40" s="2">
         <v>0.60000000133674902</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>39</v>
       </c>
@@ -40625,8 +41365,11 @@
       <c r="F41" s="2">
         <v>0.59999999919795</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>40</v>
       </c>
@@ -40645,8 +41388,11 @@
       <c r="F42" s="2">
         <v>0.60000000048123003</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>41</v>
       </c>
@@ -40665,8 +41411,11 @@
       <c r="F43" s="2">
         <v>0.59999999971126095</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>42</v>
       </c>
@@ -40685,8 +41434,11 @@
       <c r="F44" s="2">
         <v>0.60000000017324295</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>43</v>
       </c>
@@ -40705,8 +41457,11 @@
       <c r="F45" s="2">
         <v>0.59999999989605401</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>44</v>
       </c>
@@ -40725,8 +41480,11 @@
       <c r="F46" s="2">
         <v>0.60000000006236698</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H46" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>45</v>
       </c>
@@ -40745,8 +41503,11 @@
       <c r="F47" s="2">
         <v>0.59999999996257902</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H47" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>46</v>
       </c>
@@ -40765,8 +41526,11 @@
       <c r="F48" s="2">
         <v>0.60000000002245202</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>47</v>
       </c>
@@ -40785,8 +41549,11 @@
       <c r="F49" s="2">
         <v>0.59999999998652798</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>48</v>
       </c>
@@ -40805,8 +41572,11 @@
       <c r="F50" s="2">
         <v>0.60000000000808296</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H50" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>49</v>
       </c>
@@ -40825,8 +41595,11 @@
       <c r="F51" s="2">
         <v>0.59999999999514997</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H51" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>50</v>
       </c>
@@ -40845,8 +41618,11 @@
       <c r="F52" s="2">
         <v>0.92000000000290905</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H52" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>51</v>
       </c>
@@ -40865,8 +41641,11 @@
       <c r="F53" s="2">
         <v>0.72799999999825404</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H53" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>52</v>
       </c>
@@ -40885,8 +41664,11 @@
       <c r="F54" s="2">
         <v>0.843200000001047</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>53</v>
       </c>
@@ -40905,8 +41687,11 @@
       <c r="F55" s="2">
         <v>0.77407999999937105</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>54</v>
       </c>
@@ -40925,8 +41710,11 @@
       <c r="F56" s="2">
         <v>0.81555200000037698</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H56" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>55</v>
       </c>
@@ -40945,8 +41733,11 @@
       <c r="F57" s="2">
         <v>0.79066879999977302</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H57" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>56</v>
       </c>
@@ -40965,8 +41756,11 @@
       <c r="F58" s="2">
         <v>0.80559872000013599</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H58" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>57</v>
       </c>
@@ -40985,8 +41779,11 @@
       <c r="F59" s="2">
         <v>0.79664076799991801</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H59" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>58</v>
       </c>
@@ -41005,8 +41802,11 @@
       <c r="F60" s="2">
         <v>0.80201553920004898</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H60" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>59</v>
       </c>
@@ -41025,8 +41825,11 @@
       <c r="F61" s="2">
         <v>0.79879067647997004</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H61" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>60</v>
       </c>
@@ -41045,8 +41848,11 @@
       <c r="F62" s="2">
         <v>0.80072559411201705</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H62" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>61</v>
       </c>
@@ -41065,8 +41871,11 @@
       <c r="F63" s="2">
         <v>0.799564643532789</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H63" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>62</v>
       </c>
@@ -41085,8 +41894,11 @@
       <c r="F64" s="2">
         <v>0.80026121388032601</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H64" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>63</v>
       </c>
@@ -41105,8 +41917,11 @@
       <c r="F65" s="2">
         <v>0.79984327167180402</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>64</v>
       </c>
@@ -41125,8 +41940,11 @@
       <c r="F66" s="2">
         <v>0.80009403699691695</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H66" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>65</v>
       </c>
@@ -41145,8 +41963,11 @@
       <c r="F67" s="2">
         <v>0.79994357780184899</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H67" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>66</v>
       </c>
@@ -41165,8 +41986,11 @@
       <c r="F68" s="2">
         <v>0.80003385331888999</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H68" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>67</v>
       </c>
@@ -41185,8 +42009,11 @@
       <c r="F69" s="2">
         <v>0.79997968800866603</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H69" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>68</v>
       </c>
@@ -41205,8 +42032,11 @@
       <c r="F70" s="2">
         <v>0.80001218719480005</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H70" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>69</v>
       </c>
@@ -41225,8 +42055,11 @@
       <c r="F71" s="2">
         <v>0.79999268768311904</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H71" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>70</v>
       </c>
@@ -41245,8 +42078,11 @@
       <c r="F72" s="2">
         <v>0.80000438739012802</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H72" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>71</v>
       </c>
@@ -41265,8 +42101,11 @@
       <c r="F73" s="2">
         <v>0.79999736756592299</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H73" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>72</v>
       </c>
@@ -41285,8 +42124,11 @@
       <c r="F74" s="2">
         <v>0.80000157946044603</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H74" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>73</v>
       </c>
@@ -41305,8 +42147,11 @@
       <c r="F75" s="2">
         <v>0.79999905232373203</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H75" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>74</v>
       </c>
@@ -41325,8 +42170,11 @@
       <c r="F76" s="2">
         <v>0.80000056860575997</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H76" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>75</v>
       </c>
@@ -41345,8 +42193,11 @@
       <c r="F77" s="2">
         <v>0.799999658836543</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H77" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>76</v>
       </c>
@@ -41365,8 +42216,11 @@
       <c r="F78" s="2">
         <v>0.80000020469807398</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H78" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>77</v>
       </c>
@@ -41385,8 +42239,11 @@
       <c r="F79" s="2">
         <v>0.79999987718115495</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H79" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>78</v>
       </c>
@@ -41405,8 +42262,11 @@
       <c r="F80" s="2">
         <v>0.80000007369130599</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H80" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>79</v>
       </c>
@@ -41425,8 +42285,11 @@
       <c r="F81" s="2">
         <v>0.79999995578521599</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H81" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>80</v>
       </c>
@@ -41445,8 +42308,11 @@
       <c r="F82" s="2">
         <v>0.80000002652887003</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>81</v>
       </c>
@@ -41465,8 +42331,11 @@
       <c r="F83" s="2">
         <v>0.79999998408267703</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H83" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>82</v>
       </c>
@@ -41485,8 +42354,11 @@
       <c r="F84" s="2">
         <v>0.80000000955039297</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H84" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>83</v>
       </c>
@@ -41505,8 +42377,11 @@
       <c r="F85" s="2">
         <v>0.79999999426976398</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H85" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>84</v>
       </c>
@@ -41525,8 +42400,11 @@
       <c r="F86" s="2">
         <v>0.80000000343814104</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H86" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>85</v>
       </c>
@@ -41545,8 +42423,11 @@
       <c r="F87" s="2">
         <v>0.79999999793711496</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H87" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>86</v>
       </c>
@@ -41565,8 +42446,11 @@
       <c r="F88" s="2">
         <v>0.80000000123772996</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H88" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>87</v>
       </c>
@@ -41585,8 +42469,11 @@
       <c r="F89" s="2">
         <v>0.79999999925736098</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H89" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>88</v>
       </c>
@@ -41605,8 +42492,11 @@
       <c r="F90" s="2">
         <v>0.80000000044558295</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H90" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>89</v>
       </c>
@@ -41625,8 +42515,11 @@
       <c r="F91" s="2">
         <v>0.79999999973265001</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H91" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>90</v>
       </c>
@@ -41645,8 +42538,11 @@
       <c r="F92" s="2">
         <v>0.80000000016040895</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H92" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>91</v>
       </c>
@@ -41665,8 +42561,11 @@
       <c r="F93" s="2">
         <v>0.79999999990375403</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H93" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>92</v>
       </c>
@@ -41685,8 +42584,11 @@
       <c r="F94" s="2">
         <v>0.80000000005774696</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H94" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>93</v>
       </c>
@@ -41705,8 +42607,11 @@
       <c r="F95" s="2">
         <v>0.79999999996535098</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H95" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>94</v>
       </c>
@@ -41725,8 +42630,11 @@
       <c r="F96" s="2">
         <v>0.80000000002078897</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H96" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>95</v>
       </c>
@@ -41745,8 +42653,11 @@
       <c r="F97" s="2">
         <v>0.79999999998752602</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H97" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>96</v>
       </c>
@@ -41765,8 +42676,11 @@
       <c r="F98" s="2">
         <v>0.80000000000748395</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H98" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>97</v>
       </c>
@@ -41785,8 +42699,11 @@
       <c r="F99" s="2">
         <v>0.79999999999550897</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H99" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>98</v>
       </c>
@@ -41805,8 +42722,11 @@
       <c r="F100" s="2">
         <v>0.800000000002694</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H100" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>99</v>
       </c>
@@ -41825,8 +42745,11 @@
       <c r="F101" s="2">
         <v>0.799999999998383</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H101" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>100</v>
       </c>
@@ -41845,8 +42768,11 @@
       <c r="F102" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H102" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>101</v>
       </c>
@@ -41865,8 +42791,11 @@
       <c r="F103" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H103" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>102</v>
       </c>
@@ -41885,8 +42814,11 @@
       <c r="F104" s="2">
         <v>9.6980201647056601E-13</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H104" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>103</v>
       </c>
@@ -41905,8 +42837,11 @@
       <c r="F105" s="2">
         <v>0.159999999999418</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H105" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>104</v>
       </c>
@@ -41925,8 +42860,11 @@
       <c r="F106" s="2">
         <v>6.4000000000349097E-2</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H106" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>105</v>
       </c>
@@ -41945,8 +42883,11 @@
       <c r="F107" s="2">
         <v>0.12159999999979</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H107" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>106</v>
       </c>
@@ -41965,8 +42906,11 @@
       <c r="F108" s="2">
         <v>8.7040000000125697E-2</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H108" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>107</v>
       </c>
@@ -41985,8 +42929,11 @@
       <c r="F109" s="2">
         <v>0.107775999999924</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H109" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>108</v>
       </c>
@@ -42005,8 +42952,11 @@
       <c r="F110" s="2">
         <v>9.53344000000452E-2</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H110" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>109</v>
       </c>
@@ -42025,8 +42975,11 @@
       <c r="F111" s="2">
         <v>0.102799359999972</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H111" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>110</v>
       </c>
@@ -42045,8 +42998,11 @@
       <c r="F112" s="2">
         <v>9.8320384000016303E-2</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H112" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>111</v>
       </c>
@@ -42065,8 +43021,11 @@
       <c r="F113" s="2">
         <v>0.10100776959999</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H113" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>112</v>
       </c>
@@ -42085,8 +43044,11 @@
       <c r="F114" s="2">
         <v>9.9395338240005807E-2</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H114" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>113</v>
       </c>
@@ -42105,8 +43067,11 @@
       <c r="F115" s="2">
         <v>0.100362797055996</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H115" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>114</v>
       </c>
@@ -42125,8 +43090,11 @@
       <c r="F116" s="2">
         <v>9.9782321766402102E-2</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H116" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>115</v>
       </c>
@@ -42145,8 +43113,11 @@
       <c r="F117" s="2">
         <v>0.100130606940158</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H117" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>116</v>
       </c>
@@ -42165,8 +43136,11 @@
       <c r="F118" s="2">
         <v>9.9921635835904701E-2</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H118" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>117</v>
       </c>
@@ -42185,8 +43159,11 @@
       <c r="F119" s="2">
         <v>0.100047018498457</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H119" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>118</v>
       </c>
@@ -42205,8 +43182,11 @@
       <c r="F120" s="2">
         <v>9.9971788900925701E-2</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H120" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>119</v>
       </c>
@@ -42225,8 +43205,11 @@
       <c r="F121" s="2">
         <v>0.10001692665944401</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H121" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>120</v>
       </c>
@@ -42245,8 +43228,11 @@
       <c r="F122" s="2">
         <v>9.9989844004333195E-2</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H122" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>121</v>
       </c>
@@ -42265,8 +43251,11 @@
       <c r="F123" s="2">
         <v>0.10000609359739999</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H123" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>122</v>
       </c>
@@ -42285,8 +43274,11 @@
       <c r="F124" s="2">
         <v>9.9996343841559907E-2</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H124" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>123</v>
       </c>
@@ -42305,8 +43297,11 @@
       <c r="F125" s="2">
         <v>0.100002193695064</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H125" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>124</v>
       </c>
@@ -42325,8 +43320,11 @@
       <c r="F126" s="2">
         <v>9.9998683782961603E-2</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H126" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
         <v>125</v>
       </c>
@@ -42345,8 +43343,11 @@
       <c r="F127" s="2">
         <v>0.100000789730223</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H127" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
         <v>126</v>
       </c>
@@ -42365,8 +43366,11 @@
       <c r="F128" s="2">
         <v>9.9999526161866095E-2</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H128" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
         <v>127</v>
       </c>
@@ -42385,8 +43389,11 @@
       <c r="F129" s="2">
         <v>0.10000028430287999</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H129" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
         <v>128</v>
       </c>
@@ -42405,8 +43412,11 @@
       <c r="F130" s="2">
         <v>9.9999829418271804E-2</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H130" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
         <v>129</v>
       </c>
@@ -42425,8 +43435,11 @@
       <c r="F131" s="2">
         <v>0.100000102349036</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H131" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
         <v>130</v>
       </c>
@@ -42445,8 +43458,11 @@
       <c r="F132" s="2">
         <v>9.9999938590577805E-2</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H132" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
         <v>131</v>
       </c>
@@ -42465,8 +43481,11 @@
       <c r="F133" s="2">
         <v>0.10000003684565301</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H133" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
         <v>132</v>
       </c>
@@ -42485,8 +43504,11 @@
       <c r="F134" s="2">
         <v>9.9999977892608005E-2</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H134" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
         <v>133</v>
       </c>
@@ -42505,8 +43527,11 @@
       <c r="F135" s="2">
         <v>0.100000013264435</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H135" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
         <v>134</v>
       </c>
@@ -42525,8 +43550,11 @@
       <c r="F136" s="2">
         <v>9.9999992041338803E-2</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H136" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
         <v>135</v>
       </c>
@@ -42545,8 +43573,11 @@
       <c r="F137" s="2">
         <v>0.10000000477519599</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H137" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>136</v>
       </c>
@@ -42565,8 +43596,11 @@
       <c r="F138" s="2">
         <v>9.9999997134881904E-2</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H138" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
         <v>137</v>
       </c>
@@ -42585,8 +43619,11 @@
       <c r="F139" s="2">
         <v>0.10000000171907</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H139" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
         <v>138</v>
       </c>
@@ -42605,8 +43642,11 @@
       <c r="F140" s="2">
         <v>9.9999998968557505E-2</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H140" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
         <v>139</v>
       </c>
@@ -42625,8 +43665,11 @@
       <c r="F141" s="2">
         <v>0.10000000061886501</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H141" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
         <v>140</v>
       </c>
@@ -42645,8 +43688,11 @@
       <c r="F142" s="2">
         <v>9.9999999628680697E-2</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H142" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" s="2">
         <v>141</v>
       </c>
@@ -42665,8 +43711,11 @@
       <c r="F143" s="2">
         <v>0.100000000222791</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H143" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
         <v>142</v>
       </c>
@@ -42685,8 +43734,11 @@
       <c r="F144" s="2">
         <v>9.9999999866325004E-2</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H144" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
         <v>143</v>
       </c>
@@ -42705,8 +43757,11 @@
       <c r="F145" s="2">
         <v>0.100000000080204</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H145" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
         <v>144</v>
       </c>
@@ -42725,8 +43780,11 @@
       <c r="F146" s="2">
         <v>9.9999999951877E-2</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H146" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" s="2">
         <v>145</v>
       </c>
@@ -42745,8 +43803,11 @@
       <c r="F147" s="2">
         <v>0.10000000002887301</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H147" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
         <v>146</v>
       </c>
@@ -42765,8 +43826,11 @@
       <c r="F148" s="2">
         <v>9.9999999982675697E-2</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H148" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" s="2">
         <v>147</v>
       </c>
@@ -42785,8 +43849,11 @@
       <c r="F149" s="2">
         <v>0.100000000010394</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H149" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
         <v>148</v>
       </c>
@@ -42805,8 +43872,11 @@
       <c r="F150" s="2">
         <v>9.9999999993763203E-2</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H150" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" s="2">
         <v>149</v>
       </c>
@@ -42825,8 +43895,11 @@
       <c r="F151" s="2">
         <v>0.100000000003742</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H151" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" s="2">
         <v>150</v>
       </c>
@@ -42845,8 +43918,11 @@
       <c r="F152" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H152" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" s="2">
         <v>151</v>
       </c>
@@ -42865,8 +43941,11 @@
       <c r="F153" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H153" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
         <v>152</v>
       </c>
@@ -42885,8 +43964,11 @@
       <c r="F154" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H154" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" s="2">
         <v>153</v>
       </c>
@@ -42905,8 +43987,11 @@
       <c r="F155" s="2">
         <v>0.89999999999775404</v>
       </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H155" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" s="2">
         <v>154</v>
       </c>
@@ -42925,8 +44010,11 @@
       <c r="F156" s="2">
         <v>0.90000000000134694</v>
       </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H156" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" s="2">
         <v>155</v>
       </c>
@@ -42945,8 +44033,11 @@
       <c r="F157" s="2">
         <v>0.899999999999191</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H157" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" s="2">
         <v>156</v>
       </c>
@@ -42965,8 +44056,11 @@
       <c r="F158" s="2">
         <v>0.90000000000048497</v>
       </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H158" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" s="2">
         <v>157</v>
       </c>
@@ -42985,8 +44079,11 @@
       <c r="F159" s="2">
         <v>0.89999999999970803</v>
       </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H159" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" s="2">
         <v>158</v>
       </c>
@@ -43005,8 +44102,11 @@
       <c r="F160" s="2">
         <v>0.90000000000017399</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H160" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" s="2">
         <v>159</v>
       </c>
@@ -43025,8 +44125,11 @@
       <c r="F161" s="2">
         <v>0.899999999999895</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H161" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" s="2">
         <v>160</v>
       </c>
@@ -43045,8 +44148,11 @@
       <c r="F162" s="2">
         <v>0.90000000000006297</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H162" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" s="2">
         <v>161</v>
       </c>
@@ -43065,8 +44171,11 @@
       <c r="F163" s="2">
         <v>0.89999999999996205</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H163" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" s="2">
         <v>162</v>
       </c>
@@ -43085,8 +44194,11 @@
       <c r="F164" s="2">
         <v>0.900000000000022</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H164" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" s="2">
         <v>163</v>
       </c>
@@ -43105,8 +44217,11 @@
       <c r="F165" s="2">
         <v>0.89999999999998603</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H165" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" s="2">
         <v>164</v>
       </c>
@@ -43125,8 +44240,11 @@
       <c r="F166" s="2">
         <v>0.90000000000000802</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H166" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" s="2">
         <v>165</v>
       </c>
@@ -43145,8 +44263,11 @@
       <c r="F167" s="2">
         <v>0.89999999999999503</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H167" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" s="2">
         <v>166</v>
       </c>
@@ -43165,8 +44286,11 @@
       <c r="F168" s="2">
         <v>0.90000000000000302</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H168" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" s="2">
         <v>167</v>
       </c>
@@ -43185,8 +44309,11 @@
       <c r="F169" s="2">
         <v>0.89999999999999802</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H169" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" s="2">
         <v>168</v>
       </c>
@@ -43205,8 +44332,11 @@
       <c r="F170" s="2">
         <v>0.90000000000000102</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H170" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" s="2">
         <v>169</v>
       </c>
@@ -43225,8 +44355,11 @@
       <c r="F171" s="2">
         <v>0.89999999999999902</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H171" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" s="2">
         <v>170</v>
       </c>
@@ -43245,8 +44378,11 @@
       <c r="F172" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H172" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" s="2">
         <v>171</v>
       </c>
@@ -43265,8 +44401,11 @@
       <c r="F173" s="2">
         <v>0.89999999999999902</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H173" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" s="2">
         <v>172</v>
       </c>
@@ -43285,8 +44424,11 @@
       <c r="F174" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H174" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" s="2">
         <v>173</v>
       </c>
@@ -43305,8 +44447,11 @@
       <c r="F175" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H175" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" s="2">
         <v>174</v>
       </c>
@@ -43325,8 +44470,11 @@
       <c r="F176" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H176" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" s="2">
         <v>175</v>
       </c>
@@ -43345,8 +44493,11 @@
       <c r="F177" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H177" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" s="2">
         <v>176</v>
       </c>
@@ -43365,8 +44516,11 @@
       <c r="F178" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H178" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" s="2">
         <v>177</v>
       </c>
@@ -43385,8 +44539,11 @@
       <c r="F179" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H179" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" s="2">
         <v>178</v>
       </c>
@@ -43405,8 +44562,11 @@
       <c r="F180" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H180" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" s="2">
         <v>179</v>
       </c>
@@ -43425,8 +44585,11 @@
       <c r="F181" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H181" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" s="2">
         <v>180</v>
       </c>
@@ -43445,8 +44608,11 @@
       <c r="F182" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H182" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" s="2">
         <v>181</v>
       </c>
@@ -43465,8 +44631,11 @@
       <c r="F183" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H183" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" s="2">
         <v>182</v>
       </c>
@@ -43485,8 +44654,11 @@
       <c r="F184" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H184" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" s="2">
         <v>183</v>
       </c>
@@ -43505,8 +44677,11 @@
       <c r="F185" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H185" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" s="2">
         <v>184</v>
       </c>
@@ -43525,8 +44700,11 @@
       <c r="F186" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H186" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" s="2">
         <v>185</v>
       </c>
@@ -43545,8 +44723,11 @@
       <c r="F187" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H187" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" s="2">
         <v>186</v>
       </c>
@@ -43565,8 +44746,11 @@
       <c r="F188" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H188" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" s="2">
         <v>187</v>
       </c>
@@ -43585,8 +44769,11 @@
       <c r="F189" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H189" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" s="2">
         <v>188</v>
       </c>
@@ -43605,8 +44792,11 @@
       <c r="F190" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H190" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" s="2">
         <v>189</v>
       </c>
@@ -43625,8 +44815,11 @@
       <c r="F191" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H191" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" s="2">
         <v>190</v>
       </c>
@@ -43645,8 +44838,11 @@
       <c r="F192" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H192" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" s="2">
         <v>191</v>
       </c>
@@ -43665,8 +44861,11 @@
       <c r="F193" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H193" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" s="2">
         <v>192</v>
       </c>
@@ -43685,8 +44884,11 @@
       <c r="F194" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H194" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" s="2">
         <v>193</v>
       </c>
@@ -43705,8 +44907,11 @@
       <c r="F195" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H195" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" s="2">
         <v>194</v>
       </c>
@@ -43725,8 +44930,11 @@
       <c r="F196" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H196" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" s="2">
         <v>195</v>
       </c>
@@ -43745,8 +44953,11 @@
       <c r="F197" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H197" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" s="2">
         <v>196</v>
       </c>
@@ -43765,8 +44976,11 @@
       <c r="F198" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H198" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" s="2">
         <v>197</v>
       </c>
@@ -43785,8 +44999,11 @@
       <c r="F199" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H199" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" s="2">
         <v>198</v>
       </c>
@@ -43805,8 +45022,11 @@
       <c r="F200" s="2">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H200" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" s="2">
         <v>199</v>
       </c>
@@ -43824,6 +45044,9 @@
       </c>
       <c r="F201" s="2">
         <v>0.9</v>
+      </c>
+      <c r="H201" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>